<commit_message>
Update MOFC GUI Excel files
</commit_message>
<xml_diff>
--- a/MOFC_GUI_TEST1.2.xlsx
+++ b/MOFC_GUI_TEST1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyiz\Documents\Work\CDRP\MOFC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB1FBD9-04AF-47A8-9B93-2B37A5189511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FDA73F-C7CD-4264-A807-C0562C9D994E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6885" yWindow="0" windowWidth="32535" windowHeight="20040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTS" sheetId="29" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="115">
   <si>
     <t>DCA1</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t>Ch7Cfg</t>
+  </si>
+  <si>
+    <t>PM-PWIDTH[us]</t>
   </si>
 </sst>
 </file>
@@ -933,36 +936,6 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -979,6 +952,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3189,8 +3192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C2EE34-62CF-470A-B0BB-430B64842E02}">
   <dimension ref="A4:W365"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3318,7 +3321,7 @@
         <v>-32</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" ref="C7:C68" si="0">C6+125</f>
+        <f t="shared" ref="C7:C59" si="0">C6+125</f>
         <v>10250</v>
       </c>
       <c r="D7" s="5">
@@ -7721,8 +7724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AC0837-B9D8-4482-835B-7E0DD2B30E78}">
   <dimension ref="C2:AK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7786,35 +7789,35 @@
       </c>
       <c r="W3" s="51" t="str">
         <f>DEC2HEX(C11,8)</f>
-        <v>000019A0</v>
+        <v>0000C8F0</v>
       </c>
       <c r="X3" s="51" t="str">
         <f t="shared" ref="X3:X10" si="0">"0x"&amp;DEC2HEX(U3*2^24+HEX2DEC(W3),8)</f>
-        <v>0x060019A0</v>
+        <v>0x0600C8F0</v>
       </c>
       <c r="Y3" s="51">
         <f t="shared" ref="Y3:Y37" si="1">_xlfn.BITXOR(_xlfn.BITXOR(MOD(HEX2DEC(W3),256),MOD(INT(HEX2DEC(W3)/256),256)),INT(HEX2DEC(W3)/65536))</f>
-        <v>185</v>
+        <v>56</v>
       </c>
       <c r="Z3" s="51"/>
     </row>
     <row r="4" spans="3:37" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="72"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="62"/>
       <c r="T4" s="56" t="s">
         <v>98</v>
       </c>
@@ -7854,7 +7857,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="8"/>
-      <c r="T5" s="60" t="s">
+      <c r="T5" s="67" t="s">
         <v>96</v>
       </c>
       <c r="U5" s="51">
@@ -7882,27 +7885,27 @@
       </c>
     </row>
     <row r="6" spans="3:37" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="66"/>
+      <c r="D6" s="69"/>
       <c r="E6" s="13"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="73" t="s">
+      <c r="I6" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="75"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="64"/>
+      <c r="Q6" s="65"/>
       <c r="R6" s="8"/>
-      <c r="T6" s="60"/>
+      <c r="T6" s="67"/>
       <c r="U6" s="51">
         <v>9</v>
       </c>
@@ -7935,10 +7938,10 @@
         <v>89</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="69" t="s">
+      <c r="F7" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="69"/>
+      <c r="G7" s="66"/>
       <c r="H7" s="6"/>
       <c r="I7" s="14"/>
       <c r="J7" s="15">
@@ -7966,7 +7969,7 @@
         <v>8</v>
       </c>
       <c r="R7" s="8"/>
-      <c r="T7" s="60"/>
+      <c r="T7" s="67"/>
       <c r="U7" s="51">
         <v>10</v>
       </c>
@@ -8063,7 +8066,7 @@
         <v>7</v>
       </c>
       <c r="R8" s="8"/>
-      <c r="T8" s="60"/>
+      <c r="T8" s="67"/>
       <c r="U8" s="51">
         <v>11</v>
       </c>
@@ -8087,42 +8090,42 @@
         <f t="shared" ca="1" si="3"/>
         <v>17</v>
       </c>
-      <c r="AB8" s="61" t="s">
+      <c r="AB8" s="72" t="s">
         <v>103</v>
       </c>
       <c r="AC8" s="53">
         <v>0</v>
       </c>
       <c r="AD8" s="2">
-        <f>(MATCH(J8,RFISRC,0)-1)</f>
+        <f t="shared" ref="AD8:AK8" si="4">(MATCH(J8,RFISRC,0)-1)</f>
         <v>1</v>
       </c>
       <c r="AE8" s="2">
-        <f>(MATCH(K8,RFISRC,0)-1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF8" s="2">
-        <f>(MATCH(L8,RFISRC,0)-1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AG8" s="2">
-        <f>(MATCH(M8,RFISRC,0)-1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AH8" s="2">
-        <f>(MATCH(N8,RFISRC,0)-1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AI8" s="2">
-        <f>(MATCH(O8,RFISRC,0)-1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AJ8" s="2">
-        <f>(MATCH(P8,RFISRC,0)-1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AK8" s="2">
-        <f>(MATCH(Q8,RFISRC,0)-1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8132,14 +8135,14 @@
       </c>
       <c r="D9" s="1">
         <f>G9</f>
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="15" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="G9" s="14">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="29" t="s">
@@ -8170,7 +8173,7 @@
         <v>5</v>
       </c>
       <c r="R9" s="8"/>
-      <c r="T9" s="60" t="s">
+      <c r="T9" s="67" t="s">
         <v>107</v>
       </c>
       <c r="U9" s="51">
@@ -8196,40 +8199,40 @@
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="AB9" s="61"/>
+      <c r="AB9" s="72"/>
       <c r="AC9" s="53">
         <v>1</v>
       </c>
       <c r="AD9" s="2">
-        <f>(MATCH(J9,RFIBS,0)-1)</f>
+        <f t="shared" ref="AD9:AK9" si="5">(MATCH(J9,RFIBS,0)-1)</f>
         <v>1</v>
       </c>
       <c r="AE9" s="2">
-        <f>(MATCH(K9,RFIBS,0)-1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AF9" s="2">
-        <f>(MATCH(L9,RFIBS,0)-1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG9" s="2">
-        <f>(MATCH(M9,RFIBS,0)-1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AH9" s="2">
-        <f>(MATCH(N9,RFIBS,0)-1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AI9" s="2">
-        <f>(MATCH(O9,RFIBS,0)-1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="AJ9" s="2">
-        <f>(MATCH(P9,RFIBS,0)-1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AK9" s="2">
-        <f>(MATCH(Q9,RFIBS,0)-1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8239,14 +8242,14 @@
       </c>
       <c r="D10" s="1">
         <f>G10</f>
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="14">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="29" t="s">
@@ -8277,7 +8280,7 @@
         <v>2</v>
       </c>
       <c r="R10" s="8"/>
-      <c r="T10" s="60"/>
+      <c r="T10" s="67"/>
       <c r="U10" s="51">
         <v>13</v>
       </c>
@@ -8301,47 +8304,47 @@
         <f t="shared" ca="1" si="3"/>
         <v>37</v>
       </c>
-      <c r="AB10" s="61"/>
+      <c r="AB10" s="72"/>
       <c r="AC10" s="53">
         <v>3</v>
       </c>
       <c r="AD10" s="2">
-        <f>(MATCH(J10,IFOBS,0)-1)</f>
+        <f t="shared" ref="AD10:AK10" si="6">(MATCH(J10,IFOBS,0)-1)</f>
         <v>1</v>
       </c>
       <c r="AE10" s="2">
-        <f>(MATCH(K10,IFOBS,0)-1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AF10" s="2">
-        <f>(MATCH(L10,IFOBS,0)-1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AG10" s="2">
-        <f>(MATCH(M10,IFOBS,0)-1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AH10" s="2">
-        <f>(MATCH(N10,IFOBS,0)-1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AI10" s="2">
-        <f>(MATCH(O10,IFOBS,0)-1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AJ10" s="2">
-        <f>(MATCH(P10,IFOBS,0)-1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AK10" s="2">
-        <f>(MATCH(Q10,IFOBS,0)-1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <f>D8*2^C8+D9*2^C9+D10*2^C10</f>
-        <v>6560</v>
+        <v>51440</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="13"/>
@@ -8376,7 +8379,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="8"/>
-      <c r="T11" s="60"/>
+      <c r="T11" s="67"/>
       <c r="U11" s="51">
         <v>14</v>
       </c>
@@ -8389,7 +8392,7 @@
         <v>00000881</v>
       </c>
       <c r="X11" s="51" t="str">
-        <f t="shared" ref="X11:X37" ca="1" si="4">"0x"&amp;DEC2HEX(U11*2^24+HEX2DEC(W11),8)</f>
+        <f t="shared" ref="X11:X37" ca="1" si="7">"0x"&amp;DEC2HEX(U11*2^24+HEX2DEC(W11),8)</f>
         <v>0x0E000881</v>
       </c>
       <c r="Y11" s="51">
@@ -8397,43 +8400,43 @@
         <v>137</v>
       </c>
       <c r="Z11" s="51">
-        <f t="shared" ref="Z11:Z35" ca="1" si="5">_xlfn.BITXOR(Y10,Y11)</f>
+        <f t="shared" ref="Z11:Z35" ca="1" si="8">_xlfn.BITXOR(Y10,Y11)</f>
         <v>147</v>
       </c>
-      <c r="AB11" s="61"/>
+      <c r="AB11" s="72"/>
       <c r="AC11" s="53">
         <v>4</v>
       </c>
       <c r="AD11" s="2">
-        <f>(MATCH(J11,DCA,0)-1)</f>
+        <f t="shared" ref="AD11:AK13" si="9">(MATCH(J11,DCA,0)-1)</f>
         <v>2</v>
       </c>
       <c r="AE11" s="2">
-        <f>(MATCH(K11,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF11" s="2">
-        <f>(MATCH(L11,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG11" s="2">
-        <f>(MATCH(M11,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH11" s="2">
-        <f>(MATCH(N11,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI11" s="2">
-        <f>(MATCH(O11,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="2">
-        <f>(MATCH(P11,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK11" s="2">
-        <f>(MATCH(Q11,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8472,7 +8475,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="8"/>
-      <c r="T12" s="60"/>
+      <c r="T12" s="67"/>
       <c r="U12" s="51">
         <v>15</v>
       </c>
@@ -8485,7 +8488,7 @@
         <v>00000001</v>
       </c>
       <c r="X12" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x0F000001</v>
       </c>
       <c r="Y12" s="51">
@@ -8493,43 +8496,43 @@
         <v>1</v>
       </c>
       <c r="Z12" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>136</v>
       </c>
-      <c r="AB12" s="61"/>
+      <c r="AB12" s="72"/>
       <c r="AC12" s="53">
         <v>10</v>
       </c>
       <c r="AD12" s="2">
-        <f>(MATCH(J12,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AE12" s="2">
-        <f>(MATCH(K12,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AF12" s="2">
-        <f>(MATCH(L12,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG12" s="2">
-        <f>(MATCH(M12,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH12" s="2">
-        <f>(MATCH(N12,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI12" s="2">
-        <f>(MATCH(O12,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="2">
-        <f>(MATCH(P12,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK12" s="2">
-        <f>(MATCH(Q12,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8568,7 +8571,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="8"/>
-      <c r="T13" s="60" t="s">
+      <c r="T13" s="67" t="s">
         <v>108</v>
       </c>
       <c r="U13" s="51">
@@ -8583,7 +8586,7 @@
         <v>00000009</v>
       </c>
       <c r="X13" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x10000009</v>
       </c>
       <c r="Y13" s="51">
@@ -8591,43 +8594,43 @@
         <v>9</v>
       </c>
       <c r="Z13" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="AB13" s="61"/>
+      <c r="AB13" s="72"/>
       <c r="AC13" s="53">
         <v>16</v>
       </c>
       <c r="AD13" s="2">
-        <f>(MATCH(J13,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AE13" s="2">
-        <f>(MATCH(K13,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AF13" s="2">
-        <f>(MATCH(L13,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG13" s="2">
-        <f>(MATCH(M13,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH13" s="2">
-        <f>(MATCH(N13,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI13" s="2">
-        <f>(MATCH(O13,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="2">
-        <f>(MATCH(P13,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK13" s="2">
-        <f>(MATCH(Q13,DCA,0)-1)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8666,7 +8669,7 @@
         <v>62</v>
       </c>
       <c r="R14" s="8"/>
-      <c r="T14" s="60"/>
+      <c r="T14" s="67"/>
       <c r="U14" s="51">
         <v>17</v>
       </c>
@@ -8679,7 +8682,7 @@
         <v>00052B27</v>
       </c>
       <c r="X14" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x11052B27</v>
       </c>
       <c r="Y14" s="51">
@@ -8687,45 +8690,45 @@
         <v>9</v>
       </c>
       <c r="Z14" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB14" s="62" t="s">
+      <c r="AB14" s="73" t="s">
         <v>104</v>
       </c>
       <c r="AC14" s="54">
         <v>0</v>
       </c>
       <c r="AD14" s="2">
-        <f>MATCH(J14,MainBand,0)-1</f>
+        <f t="shared" ref="AD14:AK14" si="10">MATCH(J14,MainBand,0)-1</f>
         <v>2</v>
       </c>
       <c r="AE14" s="2">
-        <f>MATCH(K14,MainBand,0)-1</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AF14" s="2">
-        <f>MATCH(L14,MainBand,0)-1</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="AG14" s="2">
-        <f>MATCH(M14,MainBand,0)-1</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="AH14" s="2">
-        <f>MATCH(N14,MainBand,0)-1</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="AI14" s="2">
-        <f>MATCH(O14,MainBand,0)-1</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AJ14" s="2">
-        <f>MATCH(P14,MainBand,0)-1</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AK14" s="2">
-        <f>MATCH(Q14,MainBand,0)-1</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -8764,7 +8767,7 @@
         <v>0.52</v>
       </c>
       <c r="R15" s="8"/>
-      <c r="T15" s="60"/>
+      <c r="T15" s="67"/>
       <c r="U15" s="51">
         <v>18</v>
       </c>
@@ -8777,7 +8780,7 @@
         <v>00000481</v>
       </c>
       <c r="X15" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x12000481</v>
       </c>
       <c r="Y15" s="51">
@@ -8785,51 +8788,51 @@
         <v>133</v>
       </c>
       <c r="Z15" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>140</v>
       </c>
-      <c r="AB15" s="62"/>
+      <c r="AB15" s="73"/>
       <c r="AC15" s="54">
         <v>2</v>
       </c>
       <c r="AD15" s="2">
-        <f ca="1">MATCH(J15,INDIRECT(J14&amp;"_H"),0)</f>
+        <f t="shared" ref="AD15:AK15" ca="1" si="11">MATCH(J15,INDIRECT(J14&amp;"_H"),0)</f>
         <v>2</v>
       </c>
       <c r="AE15" s="2">
-        <f ca="1">MATCH(K15,INDIRECT(K14&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>1</v>
       </c>
       <c r="AF15" s="2">
-        <f ca="1">MATCH(L15,INDIRECT(L14&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>9</v>
       </c>
       <c r="AG15" s="2">
-        <f ca="1">MATCH(M15,INDIRECT(M14&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>3</v>
       </c>
       <c r="AH15" s="2">
-        <f ca="1">MATCH(N15,INDIRECT(N14&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>14</v>
       </c>
       <c r="AI15" s="2">
-        <f ca="1">MATCH(O15,INDIRECT(O14&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>1</v>
       </c>
       <c r="AJ15" s="2">
-        <f ca="1">MATCH(P15,INDIRECT(P14&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="AK15" s="2">
-        <f ca="1">MATCH(Q15,INDIRECT(Q14&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="66"/>
+      <c r="D16" s="69"/>
       <c r="E16" s="13"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -8862,7 +8865,7 @@
         <v>0.85</v>
       </c>
       <c r="R16" s="8"/>
-      <c r="T16" s="60"/>
+      <c r="T16" s="67"/>
       <c r="U16" s="51">
         <v>19</v>
       </c>
@@ -8875,7 +8878,7 @@
         <v>00000004</v>
       </c>
       <c r="X16" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x13000004</v>
       </c>
       <c r="Y16" s="51">
@@ -8883,43 +8886,43 @@
         <v>4</v>
       </c>
       <c r="Z16" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>129</v>
       </c>
-      <c r="AB16" s="62"/>
+      <c r="AB16" s="73"/>
       <c r="AC16" s="54">
         <v>6</v>
       </c>
       <c r="AD16" s="2">
-        <f ca="1">MATCH(J16,INDIRECT(J14&amp;"_L"),0)</f>
+        <f t="shared" ref="AD16:AK16" ca="1" si="12">MATCH(J16,INDIRECT(J14&amp;"_L"),0)</f>
         <v>5</v>
       </c>
       <c r="AE16" s="2">
-        <f ca="1">MATCH(K16,INDIRECT(K14&amp;"_L"),0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>16</v>
       </c>
       <c r="AF16" s="2">
-        <f ca="1">MATCH(L16,INDIRECT(L14&amp;"_L"),0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>12</v>
       </c>
       <c r="AG16" s="2">
-        <f ca="1">MATCH(M16,INDIRECT(M14&amp;"_L"),0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>9</v>
       </c>
       <c r="AH16" s="2">
-        <f ca="1">MATCH(N16,INDIRECT(N14&amp;"_L"),0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>14</v>
       </c>
       <c r="AI16" s="2">
-        <f ca="1">MATCH(O16,INDIRECT(O14&amp;"_L"),0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>4</v>
       </c>
       <c r="AJ16" s="2">
-        <f ca="1">MATCH(P16,INDIRECT(P14&amp;"_L"),0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>9</v>
       </c>
       <c r="AK16" s="2">
-        <f ca="1">MATCH(Q16,INDIRECT(Q14&amp;"_L"),0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>11</v>
       </c>
     </row>
@@ -8931,10 +8934,10 @@
         <v>89</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="F17" s="69" t="s">
+      <c r="F17" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="69"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="6"/>
       <c r="I17" s="31" t="s">
         <v>15</v>
@@ -8964,7 +8967,7 @@
         <v>63</v>
       </c>
       <c r="R17" s="8"/>
-      <c r="T17" s="60" t="s">
+      <c r="T17" s="67" t="s">
         <v>109</v>
       </c>
       <c r="U17" s="51">
@@ -8979,7 +8982,7 @@
         <v>0000000B</v>
       </c>
       <c r="X17" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x1400000B</v>
       </c>
       <c r="Y17" s="51">
@@ -8987,43 +8990,43 @@
         <v>11</v>
       </c>
       <c r="Z17" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="AB17" s="62"/>
+      <c r="AB17" s="73"/>
       <c r="AC17" s="54">
         <v>10</v>
       </c>
       <c r="AD17" s="2">
-        <f>MATCH(J17,MainBand,0)-1</f>
+        <f t="shared" ref="AD17:AK17" si="13">MATCH(J17,MainBand,0)-1</f>
         <v>2</v>
       </c>
       <c r="AE17" s="2">
-        <f>MATCH(K17,MainBand,0)-1</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AF17" s="2">
-        <f>MATCH(L17,MainBand,0)-1</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="AG17" s="2">
-        <f>MATCH(M17,MainBand,0)-1</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AH17" s="2">
-        <f>MATCH(N17,MainBand,0)-1</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="AI17" s="2">
-        <f>MATCH(O17,MainBand,0)-1</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="AJ17" s="2">
-        <f>MATCH(P17,MainBand,0)-1</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="AK17" s="2">
-        <f>MATCH(Q17,MainBand,0)-1</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
     </row>
@@ -9071,7 +9074,7 @@
         <v>0.95</v>
       </c>
       <c r="R18" s="8"/>
-      <c r="T18" s="60"/>
+      <c r="T18" s="67"/>
       <c r="U18" s="51">
         <v>21</v>
       </c>
@@ -9084,7 +9087,7 @@
         <v>0008264F</v>
       </c>
       <c r="X18" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x1508264F</v>
       </c>
       <c r="Y18" s="51">
@@ -9092,43 +9095,43 @@
         <v>97</v>
       </c>
       <c r="Z18" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>106</v>
       </c>
-      <c r="AB18" s="62"/>
+      <c r="AB18" s="73"/>
       <c r="AC18" s="54">
         <v>12</v>
       </c>
       <c r="AD18" s="2">
-        <f ca="1">MATCH(J18,INDIRECT(J17&amp;"_H"),0)</f>
+        <f t="shared" ref="AD18:AK18" ca="1" si="14">MATCH(J18,INDIRECT(J17&amp;"_H"),0)</f>
         <v>3</v>
       </c>
       <c r="AE18" s="2">
-        <f ca="1">MATCH(K18,INDIRECT(K17&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>1</v>
       </c>
       <c r="AF18" s="2">
-        <f ca="1">MATCH(L18,INDIRECT(L17&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>2</v>
       </c>
       <c r="AG18" s="2">
-        <f ca="1">MATCH(M18,INDIRECT(M17&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>2</v>
       </c>
       <c r="AH18" s="2">
-        <f ca="1">MATCH(N18,INDIRECT(N17&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>2</v>
       </c>
       <c r="AI18" s="2">
-        <f ca="1">MATCH(O18,INDIRECT(O17&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>2</v>
       </c>
       <c r="AJ18" s="2">
-        <f ca="1">MATCH(P18,INDIRECT(P17&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>2</v>
       </c>
       <c r="AK18" s="2">
-        <f ca="1">MATCH(Q18,INDIRECT(Q17&amp;"_H"),0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>2</v>
       </c>
     </row>
@@ -9176,7 +9179,7 @@
         <v>2.23</v>
       </c>
       <c r="R19" s="8"/>
-      <c r="T19" s="60"/>
+      <c r="T19" s="67"/>
       <c r="U19" s="51">
         <v>22</v>
       </c>
@@ -9189,7 +9192,7 @@
         <v>00000489</v>
       </c>
       <c r="X19" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x16000489</v>
       </c>
       <c r="Y19" s="51">
@@ -9197,43 +9200,43 @@
         <v>141</v>
       </c>
       <c r="Z19" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>236</v>
       </c>
-      <c r="AB19" s="62"/>
+      <c r="AB19" s="73"/>
       <c r="AC19" s="54">
         <v>16</v>
       </c>
       <c r="AD19" s="2">
-        <f ca="1">MATCH(J19,INDIRECT(J17&amp;"_L"),0)-1</f>
+        <f t="shared" ref="AD19:AK19" ca="1" si="15">MATCH(J19,INDIRECT(J17&amp;"_L"),0)-1</f>
         <v>0</v>
       </c>
       <c r="AE19" s="2">
-        <f ca="1">MATCH(K19,INDIRECT(K17&amp;"_L"),0)-1</f>
+        <f t="shared" ca="1" si="15"/>
         <v>4</v>
       </c>
       <c r="AF19" s="2">
-        <f ca="1">MATCH(L19,INDIRECT(L17&amp;"_L"),0)-1</f>
+        <f t="shared" ca="1" si="15"/>
         <v>5</v>
       </c>
       <c r="AG19" s="2">
-        <f ca="1">MATCH(M19,INDIRECT(M17&amp;"_L"),0)-1</f>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="AH19" s="2">
-        <f ca="1">MATCH(N19,INDIRECT(N17&amp;"_L"),0)-1</f>
+        <f t="shared" ca="1" si="15"/>
         <v>9</v>
       </c>
       <c r="AI19" s="2">
-        <f ca="1">MATCH(O19,INDIRECT(O17&amp;"_L"),0)-1</f>
+        <f t="shared" ca="1" si="15"/>
         <v>10</v>
       </c>
       <c r="AJ19" s="2">
-        <f ca="1">MATCH(P19,INDIRECT(P17&amp;"_L"),0)-1</f>
+        <f t="shared" ca="1" si="15"/>
         <v>9</v>
       </c>
       <c r="AK19" s="2">
-        <f ca="1">MATCH(Q19,INDIRECT(Q17&amp;"_L"),0)-1</f>
+        <f t="shared" ca="1" si="15"/>
         <v>12</v>
       </c>
     </row>
@@ -9281,7 +9284,7 @@
         <v>70</v>
       </c>
       <c r="R20" s="8"/>
-      <c r="T20" s="60"/>
+      <c r="T20" s="67"/>
       <c r="U20" s="51">
         <v>23</v>
       </c>
@@ -9294,7 +9297,7 @@
         <v>00000002</v>
       </c>
       <c r="X20" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x17000002</v>
       </c>
       <c r="Y20" s="51">
@@ -9302,45 +9305,45 @@
         <v>2</v>
       </c>
       <c r="Z20" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>143</v>
       </c>
-      <c r="AB20" s="63" t="s">
+      <c r="AB20" s="74" t="s">
         <v>105</v>
       </c>
       <c r="AC20" s="2">
         <v>0</v>
       </c>
       <c r="AD20" s="2">
-        <f>(MATCH(J20,TF2_HPF_SW,0)-1)</f>
+        <f t="shared" ref="AD20:AK20" si="16">(MATCH(J20,TF2_HPF_SW,0)-1)</f>
         <v>1</v>
       </c>
       <c r="AE20" s="2">
-        <f>(MATCH(K20,TF2_HPF_SW,0)-1)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AF20" s="2">
-        <f>(MATCH(L20,TF2_HPF_SW,0)-1)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AG20" s="2">
-        <f>(MATCH(M20,TF2_HPF_SW,0)-1)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AH20" s="2">
-        <f>(MATCH(N20,TF2_HPF_SW,0)-1)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AI20" s="2">
-        <f>(MATCH(O20,TF2_HPF_SW,0)-1)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AJ20" s="2">
-        <f>(MATCH(P20,TF2_HPF_SW,0)-1)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AK20" s="2">
-        <f>(MATCH(Q20,TF2_HPF_SW,0)-1)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
     </row>
@@ -9388,7 +9391,7 @@
         <v>1.75</v>
       </c>
       <c r="R21" s="8"/>
-      <c r="T21" s="60" t="s">
+      <c r="T21" s="67" t="s">
         <v>110</v>
       </c>
       <c r="U21" s="51">
@@ -9403,7 +9406,7 @@
         <v>0000000B</v>
       </c>
       <c r="X21" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x1800000B</v>
       </c>
       <c r="Y21" s="51">
@@ -9411,43 +9414,43 @@
         <v>11</v>
       </c>
       <c r="Z21" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="AB21" s="63"/>
+      <c r="AB21" s="74"/>
       <c r="AC21" s="2">
         <v>3</v>
       </c>
       <c r="AD21" s="2">
-        <f ca="1">MATCH(J21,INDIRECT(J20),0)-1</f>
+        <f t="shared" ref="AD21:AK21" ca="1" si="17">MATCH(J21,INDIRECT(J20),0)-1</f>
         <v>3</v>
       </c>
       <c r="AE21" s="2">
-        <f ca="1">MATCH(K21,INDIRECT(K20),0)-1</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
       <c r="AF21" s="2">
-        <f ca="1">MATCH(L21,INDIRECT(L20),0)-1</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
       <c r="AG21" s="2">
-        <f ca="1">MATCH(M21,INDIRECT(M20),0)-1</f>
+        <f t="shared" ca="1" si="17"/>
         <v>1</v>
       </c>
       <c r="AH21" s="2">
-        <f ca="1">MATCH(N21,INDIRECT(N20),0)-1</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
       <c r="AI21" s="2">
-        <f ca="1">MATCH(O21,INDIRECT(O20),0)-1</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
       <c r="AJ21" s="2">
-        <f ca="1">MATCH(P21,INDIRECT(P20),0)-1</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
       <c r="AK21" s="2">
-        <f ca="1">MATCH(Q21,INDIRECT(Q20),0)-1</f>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -9489,7 +9492,7 @@
         <v>74</v>
       </c>
       <c r="R22" s="8"/>
-      <c r="T22" s="60"/>
+      <c r="T22" s="67"/>
       <c r="U22" s="51">
         <v>25</v>
       </c>
@@ -9502,7 +9505,7 @@
         <v>00092BBB</v>
       </c>
       <c r="X22" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x19092BBB</v>
       </c>
       <c r="Y22" s="51">
@@ -9510,43 +9513,43 @@
         <v>153</v>
       </c>
       <c r="Z22" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>146</v>
       </c>
-      <c r="AB22" s="63"/>
+      <c r="AB22" s="74"/>
       <c r="AC22" s="2">
         <v>7</v>
       </c>
       <c r="AD22" s="2">
-        <f>(MATCH(J22,TF2_LPF_SW,0)-1)</f>
+        <f t="shared" ref="AD22:AK22" si="18">(MATCH(J22,TF2_LPF_SW,0)-1)</f>
         <v>2</v>
       </c>
       <c r="AE22" s="2">
-        <f>(MATCH(K22,TF2_LPF_SW,0)-1)</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="AF22" s="2">
-        <f>(MATCH(L22,TF2_LPF_SW,0)-1)</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="AG22" s="2">
-        <f>(MATCH(M22,TF2_LPF_SW,0)-1)</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="AH22" s="2">
-        <f>(MATCH(N22,TF2_LPF_SW,0)-1)</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="AI22" s="2">
-        <f>(MATCH(O22,TF2_LPF_SW,0)-1)</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="AJ22" s="2">
-        <f>(MATCH(P22,TF2_LPF_SW,0)-1)</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="AK22" s="2">
-        <f>(MATCH(Q22,TF2_LPF_SW,0)-1)</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -9585,7 +9588,7 @@
         <v>2.17</v>
       </c>
       <c r="R23" s="8"/>
-      <c r="T23" s="60"/>
+      <c r="T23" s="67"/>
       <c r="U23" s="51">
         <v>26</v>
       </c>
@@ -9598,7 +9601,7 @@
         <v>00000481</v>
       </c>
       <c r="X23" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x1A000481</v>
       </c>
       <c r="Y23" s="51">
@@ -9606,43 +9609,43 @@
         <v>133</v>
       </c>
       <c r="Z23" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>28</v>
       </c>
-      <c r="AB23" s="63"/>
+      <c r="AB23" s="74"/>
       <c r="AC23" s="2">
         <v>10</v>
       </c>
       <c r="AD23" s="2">
-        <f ca="1">MATCH(J23,INDIRECT(J22),0)-1</f>
+        <f t="shared" ref="AD23:AK23" ca="1" si="19">MATCH(J23,INDIRECT(J22),0)-1</f>
         <v>2</v>
       </c>
       <c r="AE23" s="2">
-        <f ca="1">MATCH(K23,INDIRECT(K22),0)-1</f>
+        <f t="shared" ca="1" si="19"/>
         <v>2</v>
       </c>
       <c r="AF23" s="2">
-        <f ca="1">MATCH(L23,INDIRECT(L22),0)-1</f>
+        <f t="shared" ca="1" si="19"/>
         <v>1</v>
       </c>
       <c r="AG23" s="2">
-        <f ca="1">MATCH(M23,INDIRECT(M22),0)-1</f>
+        <f t="shared" ca="1" si="19"/>
         <v>1</v>
       </c>
       <c r="AH23" s="2">
-        <f ca="1">MATCH(N23,INDIRECT(N22),0)-1</f>
+        <f t="shared" ca="1" si="19"/>
         <v>1</v>
       </c>
       <c r="AI23" s="2">
-        <f ca="1">MATCH(O23,INDIRECT(O22),0)-1</f>
+        <f t="shared" ca="1" si="19"/>
         <v>1</v>
       </c>
       <c r="AJ23" s="2">
-        <f ca="1">MATCH(P23,INDIRECT(P22),0)-1</f>
+        <f t="shared" ca="1" si="19"/>
         <v>1</v>
       </c>
       <c r="AK23" s="2">
-        <f ca="1">MATCH(Q23,INDIRECT(Q22),0)-1</f>
+        <f t="shared" ca="1" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -9681,7 +9684,7 @@
         <v>10000</v>
       </c>
       <c r="R24" s="8"/>
-      <c r="T24" s="60"/>
+      <c r="T24" s="67"/>
       <c r="U24" s="51">
         <v>27</v>
       </c>
@@ -9694,7 +9697,7 @@
         <v>00000006</v>
       </c>
       <c r="X24" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x1B000006</v>
       </c>
       <c r="Y24" s="51">
@@ -9702,45 +9705,45 @@
         <v>6</v>
       </c>
       <c r="Z24" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>131</v>
       </c>
-      <c r="AB24" s="64" t="s">
+      <c r="AB24" s="75" t="s">
         <v>106</v>
       </c>
       <c r="AC24" s="2">
         <v>0</v>
       </c>
       <c r="AD24" s="2">
-        <f>MATCH(J24,LO_FREQ,0)-1</f>
+        <f t="shared" ref="AD24:AK24" si="20">MATCH(J24,LO_FREQ,0)-1</f>
         <v>1</v>
       </c>
       <c r="AE24" s="2">
-        <f>MATCH(K24,LO_FREQ,0)-1</f>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AF24" s="2">
-        <f>MATCH(L24,LO_FREQ,0)-1</f>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="AG24" s="2">
-        <f>MATCH(M24,LO_FREQ,0)-1</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="AH24" s="2">
-        <f>MATCH(N24,LO_FREQ,0)-1</f>
+        <f t="shared" si="20"/>
         <v>6</v>
       </c>
       <c r="AI24" s="2">
-        <f>MATCH(O24,LO_FREQ,0)-1</f>
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
       <c r="AJ24" s="2">
-        <f>MATCH(P24,LO_FREQ,0)-1</f>
+        <f t="shared" si="20"/>
         <v>6</v>
       </c>
       <c r="AK24" s="2">
-        <f>MATCH(Q24,LO_FREQ,0)-1</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -9777,7 +9780,7 @@
         <v>0</v>
       </c>
       <c r="R25" s="8"/>
-      <c r="T25" s="60" t="s">
+      <c r="T25" s="67" t="s">
         <v>111</v>
       </c>
       <c r="U25" s="51">
@@ -9792,7 +9795,7 @@
         <v>0000000D</v>
       </c>
       <c r="X25" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x1C00000D</v>
       </c>
       <c r="Y25" s="51">
@@ -9800,43 +9803,43 @@
         <v>13</v>
       </c>
       <c r="Z25" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
-      <c r="AB25" s="64"/>
+      <c r="AB25" s="75"/>
       <c r="AC25" s="2">
         <v>8</v>
       </c>
       <c r="AD25" s="2">
-        <f t="shared" ref="AD25:AK25" si="6">J25</f>
+        <f t="shared" ref="AD25:AK25" si="21">J25</f>
         <v>0</v>
       </c>
       <c r="AE25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AF25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AG25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AH25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AI25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AJ25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AK25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -9855,7 +9858,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="8"/>
-      <c r="T26" s="60"/>
+      <c r="T26" s="67"/>
       <c r="U26" s="51">
         <v>29</v>
       </c>
@@ -9868,7 +9871,7 @@
         <v>000A2905</v>
       </c>
       <c r="X26" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x1D0A2905</v>
       </c>
       <c r="Y26" s="51">
@@ -9876,7 +9879,7 @@
         <v>38</v>
       </c>
       <c r="Z26" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>43</v>
       </c>
     </row>
@@ -9895,7 +9898,7 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="8"/>
-      <c r="T27" s="60"/>
+      <c r="T27" s="67"/>
       <c r="U27" s="51">
         <v>30</v>
       </c>
@@ -9908,7 +9911,7 @@
         <v>00000481</v>
       </c>
       <c r="X27" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x1E000481</v>
       </c>
       <c r="Y27" s="51">
@@ -9916,43 +9919,43 @@
         <v>133</v>
       </c>
       <c r="Z27" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>163</v>
       </c>
-      <c r="AB27" s="60" t="s">
+      <c r="AB27" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="AC27" s="60"/>
+      <c r="AC27" s="67"/>
       <c r="AD27" s="2">
-        <f t="shared" ref="AD27:AK27" si="7">AD8*2^$AC8+AD9*2^$AC9+AD10*2^$AC10+AD11*2^$AC11+AD12*2^$AC12+AD13*2^$AC13</f>
+        <f t="shared" ref="AD27:AK27" si="22">AD8*2^$AC8+AD9*2^$AC9+AD10*2^$AC10+AD11*2^$AC11+AD12*2^$AC12+AD13*2^$AC13</f>
         <v>531499</v>
       </c>
       <c r="AE27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="22"/>
         <v>531499</v>
       </c>
       <c r="AF27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="22"/>
         <v>9</v>
       </c>
       <c r="AG27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="22"/>
         <v>11</v>
       </c>
       <c r="AH27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="22"/>
         <v>11</v>
       </c>
       <c r="AI27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="22"/>
         <v>13</v>
       </c>
       <c r="AJ27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="22"/>
         <v>9</v>
       </c>
       <c r="AK27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="22"/>
         <v>9</v>
       </c>
     </row>
@@ -9971,7 +9974,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="8"/>
-      <c r="T28" s="60"/>
+      <c r="T28" s="67"/>
       <c r="U28" s="51">
         <v>31</v>
       </c>
@@ -9984,7 +9987,7 @@
         <v>00000005</v>
       </c>
       <c r="X28" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x1F000005</v>
       </c>
       <c r="Y28" s="51">
@@ -9992,43 +9995,43 @@
         <v>5</v>
       </c>
       <c r="Z28" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>128</v>
       </c>
-      <c r="AB28" s="60" t="s">
+      <c r="AB28" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="AC28" s="60"/>
+      <c r="AC28" s="67"/>
       <c r="AD28" s="2">
-        <f t="shared" ref="AD28:AK28" ca="1" si="8">AD14*2^$AC14+AD15*2^$AC15+AD16*2^$AC16+AD17*2^$AC17+AD18*2^$AC18+AD19*2^$AC19</f>
+        <f t="shared" ref="AD28:AK28" ca="1" si="23">AD14*2^$AC14+AD15*2^$AC15+AD16*2^$AC16+AD17*2^$AC17+AD18*2^$AC18+AD19*2^$AC19</f>
         <v>14666</v>
       </c>
       <c r="AE28" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="23"/>
         <v>268294</v>
       </c>
       <c r="AF28" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="23"/>
         <v>338727</v>
       </c>
       <c r="AG28" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="23"/>
         <v>534095</v>
       </c>
       <c r="AH28" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="23"/>
         <v>601019</v>
       </c>
       <c r="AI28" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="23"/>
         <v>665861</v>
       </c>
       <c r="AJ28" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="23"/>
         <v>600665</v>
       </c>
       <c r="AK28" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="23"/>
         <v>797417</v>
       </c>
     </row>
@@ -10047,7 +10050,7 @@
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
       <c r="R29" s="9"/>
-      <c r="T29" s="60" t="s">
+      <c r="T29" s="67" t="s">
         <v>112</v>
       </c>
       <c r="U29" s="51">
@@ -10062,7 +10065,7 @@
         <v>00000009</v>
       </c>
       <c r="X29" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x20000009</v>
       </c>
       <c r="Y29" s="51">
@@ -10070,49 +10073,49 @@
         <v>9</v>
       </c>
       <c r="Z29" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="AB29" s="60" t="s">
+      <c r="AB29" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="AC29" s="60"/>
+      <c r="AC29" s="67"/>
       <c r="AD29" s="2">
-        <f t="shared" ref="AD29:AK29" ca="1" si="9">AD20*2^$AC20+AD21*2^$AC21+AD22*2^$AC22+AD23*2^$AC23</f>
+        <f t="shared" ref="AD29:AK29" ca="1" si="24">AD20*2^$AC20+AD21*2^$AC21+AD22*2^$AC22+AD23*2^$AC23</f>
         <v>2329</v>
       </c>
       <c r="AE29" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="24"/>
         <v>2177</v>
       </c>
       <c r="AF29" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="24"/>
         <v>1153</v>
       </c>
       <c r="AG29" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="24"/>
         <v>1161</v>
       </c>
       <c r="AH29" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="24"/>
         <v>1153</v>
       </c>
       <c r="AI29" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="24"/>
         <v>1153</v>
       </c>
       <c r="AJ29" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="24"/>
         <v>1153</v>
       </c>
       <c r="AK29" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="24"/>
         <v>1153</v>
       </c>
     </row>
     <row r="30" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="E30" s="67"/>
-      <c r="F30" s="68"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="71"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
       <c r="I30" s="17"/>
@@ -10125,7 +10128,7 @@
       <c r="P30" s="18"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="19"/>
-      <c r="T30" s="60"/>
+      <c r="T30" s="67"/>
       <c r="U30" s="51">
         <v>33</v>
       </c>
@@ -10138,7 +10141,7 @@
         <v>00092A59</v>
       </c>
       <c r="X30" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x21092A59</v>
       </c>
       <c r="Y30" s="51">
@@ -10146,43 +10149,43 @@
         <v>122</v>
       </c>
       <c r="Z30" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>115</v>
       </c>
-      <c r="AB30" s="60" t="s">
+      <c r="AB30" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="AC30" s="60"/>
+      <c r="AC30" s="67"/>
       <c r="AD30" s="2">
-        <f t="shared" ref="AD30:AK30" si="10">AD24*2^$AC24+AD25*2^$AC25</f>
+        <f t="shared" ref="AD30:AK30" si="25">AD24*2^$AC24+AD25*2^$AC25</f>
         <v>1</v>
       </c>
       <c r="AE30" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="AF30" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="AG30" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="AH30" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>6</v>
       </c>
       <c r="AI30" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>5</v>
       </c>
       <c r="AJ30" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>6</v>
       </c>
       <c r="AK30" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -10201,7 +10204,7 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="8"/>
-      <c r="T31" s="60"/>
+      <c r="T31" s="67"/>
       <c r="U31" s="51">
         <v>34</v>
       </c>
@@ -10214,7 +10217,7 @@
         <v>00000481</v>
       </c>
       <c r="X31" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x22000481</v>
       </c>
       <c r="Y31" s="51">
@@ -10222,7 +10225,7 @@
         <v>133</v>
       </c>
       <c r="Z31" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>255</v>
       </c>
     </row>
@@ -10241,7 +10244,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="8"/>
-      <c r="T32" s="60"/>
+      <c r="T32" s="67"/>
       <c r="U32" s="51">
         <v>35</v>
       </c>
@@ -10254,7 +10257,7 @@
         <v>00000006</v>
       </c>
       <c r="X32" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x23000006</v>
       </c>
       <c r="Y32" s="51">
@@ -10262,7 +10265,7 @@
         <v>6</v>
       </c>
       <c r="Z32" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>131</v>
       </c>
     </row>
@@ -10285,7 +10288,7 @@
         <v>40</v>
       </c>
       <c r="R33" s="8"/>
-      <c r="T33" s="60" t="s">
+      <c r="T33" s="67" t="s">
         <v>113</v>
       </c>
       <c r="U33" s="51">
@@ -10300,7 +10303,7 @@
         <v>00000009</v>
       </c>
       <c r="X33" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x24000009</v>
       </c>
       <c r="Y33" s="51">
@@ -10308,7 +10311,7 @@
         <v>9</v>
       </c>
       <c r="Z33" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
     </row>
@@ -10327,7 +10330,7 @@
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
       <c r="R34" s="9"/>
-      <c r="T34" s="60"/>
+      <c r="T34" s="67"/>
       <c r="U34" s="51">
         <v>37</v>
       </c>
@@ -10340,7 +10343,7 @@
         <v>000C2AE9</v>
       </c>
       <c r="X34" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x250C2AE9</v>
       </c>
       <c r="Y34" s="51">
@@ -10348,16 +10351,16 @@
         <v>207</v>
       </c>
       <c r="Z34" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>198</v>
       </c>
     </row>
     <row r="35" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="E35" s="67" t="s">
+      <c r="E35" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
       <c r="H35" s="18"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
@@ -10369,7 +10372,7 @@
       <c r="P35" s="18"/>
       <c r="Q35" s="18"/>
       <c r="R35" s="19"/>
-      <c r="T35" s="60"/>
+      <c r="T35" s="67"/>
       <c r="U35" s="51">
         <v>38</v>
       </c>
@@ -10382,7 +10385,7 @@
         <v>00000481</v>
       </c>
       <c r="X35" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x26000481</v>
       </c>
       <c r="Y35" s="51">
@@ -10390,7 +10393,7 @@
         <v>133</v>
       </c>
       <c r="Z35" s="51">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="8"/>
         <v>74</v>
       </c>
     </row>
@@ -10409,7 +10412,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="8"/>
-      <c r="T36" s="60"/>
+      <c r="T36" s="67"/>
       <c r="U36" s="51">
         <v>39</v>
       </c>
@@ -10422,7 +10425,7 @@
         <v>00000000</v>
       </c>
       <c r="X36" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0x27000000</v>
       </c>
       <c r="Y36" s="51">
@@ -10472,7 +10475,7 @@
         <v>00000085</v>
       </c>
       <c r="X37" s="51" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0x28000085</v>
       </c>
       <c r="Y37" s="51">
@@ -10523,11 +10526,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="E4:R4"/>
-    <mergeCell ref="I6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="T25:T28"/>
-    <mergeCell ref="T29:T32"/>
+    <mergeCell ref="AB28:AC28"/>
+    <mergeCell ref="AB29:AC29"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AB8:AB13"/>
+    <mergeCell ref="AB14:AB19"/>
+    <mergeCell ref="AB20:AB23"/>
+    <mergeCell ref="AB24:AB25"/>
+    <mergeCell ref="AB27:AC27"/>
     <mergeCell ref="T33:T36"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C16:D16"/>
@@ -10539,16 +10545,13 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="AB28:AC28"/>
-    <mergeCell ref="AB29:AC29"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="AB8:AB13"/>
-    <mergeCell ref="AB14:AB19"/>
-    <mergeCell ref="AB20:AB23"/>
-    <mergeCell ref="AB24:AB25"/>
-    <mergeCell ref="AB27:AC27"/>
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="I6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="T25:T28"/>
+    <mergeCell ref="T29:T32"/>
   </mergeCells>
-  <dataValidations count="17">
+  <dataValidations count="19">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:Q8" xr:uid="{58ED200F-81A6-414B-9D6E-12786A48A800}">
       <formula1>RFISRC</formula1>
     </dataValidation>
@@ -10600,6 +10603,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18" xr:uid="{2F163C71-0122-4953-9B77-EEE0D6179D2E}">
       <formula1>BIT_LO_FREQ</formula1>
     </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9" xr:uid="{128CD636-E723-4213-908B-4E8587211284}">
+      <formula1>1</formula1>
+      <formula2>63</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10" xr:uid="{BEABB222-9253-481C-9740-F6A9D782B4E9}">
+      <formula1>G9*2</formula1>
+      <formula2>4095</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -10630,22 +10641,22 @@
   <sheetData>
     <row r="2" spans="5:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="5:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="72"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="62"/>
     </row>
     <row r="4" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E4" s="13"/>
@@ -10668,17 +10679,17 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="73" t="s">
+      <c r="I5" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="75"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="65"/>
       <c r="R5" s="33"/>
     </row>
     <row r="6" spans="5:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add all new files
</commit_message>
<xml_diff>
--- a/MOFC_GUI_TEST1.2.xlsx
+++ b/MOFC_GUI_TEST1.2.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyiz\Documents\Work\CDRP\MOFC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FDA73F-C7CD-4264-A807-C0562C9D994E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB79FB22-35A7-4518-98E9-A41DD33A6051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6885" yWindow="0" windowWidth="32535" windowHeight="20040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19335" yWindow="975" windowWidth="32535" windowHeight="20040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTS" sheetId="29" r:id="rId1"/>
@@ -524,7 +524,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,6 +586,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -788,7 +794,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -936,6 +942,36 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -952,36 +988,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1005,6 +1011,9 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1027,6 +1036,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1370,7 +1383,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3203282" y="3798793"/>
+          <a:off x="3221211" y="4323789"/>
           <a:ext cx="1054953" cy="504266"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -2746,6 +2759,108 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>19049</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1219200</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>66674</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2054" name="Button 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2054"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-IL" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:ea typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>SendMessage and</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-IL" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:ea typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>LoadRF</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-IL" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:ea typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Load</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -3190,6 +3305,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C2EE34-62CF-470A-B0BB-430B64842E02}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A4:W365"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -7721,11 +7837,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AC0837-B9D8-4482-835B-7E0DD2B30E78}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AC0837-B9D8-4482-835B-7E0DD2B30E78}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="C2:AK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7802,22 +7919,22 @@
       <c r="Z3" s="51"/>
     </row>
     <row r="4" spans="3:37" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
-      <c r="R4" s="62"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="72"/>
       <c r="T4" s="56" t="s">
         <v>98</v>
       </c>
@@ -7857,7 +7974,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="8"/>
-      <c r="T5" s="67" t="s">
+      <c r="T5" s="60" t="s">
         <v>96</v>
       </c>
       <c r="U5" s="51">
@@ -7885,27 +8002,27 @@
       </c>
     </row>
     <row r="6" spans="3:37" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="69"/>
+      <c r="D6" s="66"/>
       <c r="E6" s="13"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="63" t="s">
+      <c r="I6" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="65"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="75"/>
       <c r="R6" s="8"/>
-      <c r="T6" s="67"/>
+      <c r="T6" s="60"/>
       <c r="U6" s="51">
         <v>9</v>
       </c>
@@ -7915,19 +8032,19 @@
       </c>
       <c r="W6" s="51" t="str">
         <f ca="1">DEC2HEX(AD28,8)</f>
-        <v>0000394A</v>
+        <v>000038C9</v>
       </c>
       <c r="X6" s="51" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>0x0900394A</v>
+        <v>0x090038C9</v>
       </c>
       <c r="Y6" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>115</v>
+        <v>241</v>
       </c>
       <c r="Z6" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>76</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="3:37" ht="18.75" x14ac:dyDescent="0.25">
@@ -7938,10 +8055,10 @@
         <v>89</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="66"/>
+      <c r="G7" s="69"/>
       <c r="H7" s="6"/>
       <c r="I7" s="14"/>
       <c r="J7" s="15">
@@ -7969,7 +8086,7 @@
         <v>8</v>
       </c>
       <c r="R7" s="8"/>
-      <c r="T7" s="67"/>
+      <c r="T7" s="60"/>
       <c r="U7" s="51">
         <v>10</v>
       </c>
@@ -7991,7 +8108,7 @@
       </c>
       <c r="Z7" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>99</v>
+        <v>225</v>
       </c>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2" t="s">
@@ -8066,7 +8183,7 @@
         <v>7</v>
       </c>
       <c r="R8" s="8"/>
-      <c r="T8" s="67"/>
+      <c r="T8" s="60"/>
       <c r="U8" s="51">
         <v>11</v>
       </c>
@@ -8086,11 +8203,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Z8" s="51">
+      <c r="Z8" s="83">
         <f t="shared" ca="1" si="3"/>
         <v>17</v>
       </c>
-      <c r="AB8" s="72" t="s">
+      <c r="AB8" s="61" t="s">
         <v>103</v>
       </c>
       <c r="AC8" s="53">
@@ -8173,7 +8290,7 @@
         <v>5</v>
       </c>
       <c r="R9" s="8"/>
-      <c r="T9" s="67" t="s">
+      <c r="T9" s="60" t="s">
         <v>107</v>
       </c>
       <c r="U9" s="51">
@@ -8199,7 +8316,7 @@
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="AB9" s="72"/>
+      <c r="AB9" s="61"/>
       <c r="AC9" s="53">
         <v>1</v>
       </c>
@@ -8280,7 +8397,7 @@
         <v>2</v>
       </c>
       <c r="R10" s="8"/>
-      <c r="T10" s="67"/>
+      <c r="T10" s="60"/>
       <c r="U10" s="51">
         <v>13</v>
       </c>
@@ -8304,7 +8421,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>37</v>
       </c>
-      <c r="AB10" s="72"/>
+      <c r="AB10" s="61"/>
       <c r="AC10" s="53">
         <v>3</v>
       </c>
@@ -8379,7 +8496,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="8"/>
-      <c r="T11" s="67"/>
+      <c r="T11" s="60"/>
       <c r="U11" s="51">
         <v>14</v>
       </c>
@@ -8403,7 +8520,7 @@
         <f t="shared" ref="Z11:Z35" ca="1" si="8">_xlfn.BITXOR(Y10,Y11)</f>
         <v>147</v>
       </c>
-      <c r="AB11" s="72"/>
+      <c r="AB11" s="61"/>
       <c r="AC11" s="53">
         <v>4</v>
       </c>
@@ -8475,7 +8592,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="8"/>
-      <c r="T12" s="67"/>
+      <c r="T12" s="60"/>
       <c r="U12" s="51">
         <v>15</v>
       </c>
@@ -8495,11 +8612,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Z12" s="51">
+      <c r="Z12" s="83">
         <f t="shared" ca="1" si="8"/>
         <v>136</v>
       </c>
-      <c r="AB12" s="72"/>
+      <c r="AB12" s="61"/>
       <c r="AC12" s="53">
         <v>10</v>
       </c>
@@ -8571,7 +8688,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="8"/>
-      <c r="T13" s="67" t="s">
+      <c r="T13" s="60" t="s">
         <v>108</v>
       </c>
       <c r="U13" s="51">
@@ -8597,7 +8714,7 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="AB13" s="72"/>
+      <c r="AB13" s="61"/>
       <c r="AC13" s="53">
         <v>16</v>
       </c>
@@ -8645,7 +8762,7 @@
         <v>10</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>63</v>
@@ -8669,7 +8786,7 @@
         <v>62</v>
       </c>
       <c r="R14" s="8"/>
-      <c r="T14" s="67"/>
+      <c r="T14" s="60"/>
       <c r="U14" s="51">
         <v>17</v>
       </c>
@@ -8693,7 +8810,7 @@
         <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB14" s="73" t="s">
+      <c r="AB14" s="62" t="s">
         <v>104</v>
       </c>
       <c r="AC14" s="54">
@@ -8701,7 +8818,7 @@
       </c>
       <c r="AD14" s="2">
         <f t="shared" ref="AD14:AK14" si="10">MATCH(J14,MainBand,0)-1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE14" s="2">
         <f t="shared" si="10"/>
@@ -8743,7 +8860,7 @@
         <v>12</v>
       </c>
       <c r="J15" s="3">
-        <v>0.95</v>
+        <v>0.39</v>
       </c>
       <c r="K15" s="3">
         <v>0.93</v>
@@ -8767,7 +8884,7 @@
         <v>0.52</v>
       </c>
       <c r="R15" s="8"/>
-      <c r="T15" s="67"/>
+      <c r="T15" s="60"/>
       <c r="U15" s="51">
         <v>18</v>
       </c>
@@ -8791,7 +8908,7 @@
         <f t="shared" ca="1" si="8"/>
         <v>140</v>
       </c>
-      <c r="AB15" s="73"/>
+      <c r="AB15" s="62"/>
       <c r="AC15" s="54">
         <v>2</v>
       </c>
@@ -8829,10 +8946,10 @@
       </c>
     </row>
     <row r="16" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="69"/>
+      <c r="D16" s="66"/>
       <c r="E16" s="13"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -8841,7 +8958,7 @@
         <v>11</v>
       </c>
       <c r="J16" s="3">
-        <v>1.69</v>
+        <v>0.65</v>
       </c>
       <c r="K16" s="3">
         <v>2.6</v>
@@ -8865,7 +8982,7 @@
         <v>0.85</v>
       </c>
       <c r="R16" s="8"/>
-      <c r="T16" s="67"/>
+      <c r="T16" s="60"/>
       <c r="U16" s="51">
         <v>19</v>
       </c>
@@ -8889,13 +9006,13 @@
         <f t="shared" ca="1" si="8"/>
         <v>129</v>
       </c>
-      <c r="AB16" s="73"/>
+      <c r="AB16" s="62"/>
       <c r="AC16" s="54">
         <v>6</v>
       </c>
       <c r="AD16" s="2">
         <f t="shared" ref="AD16:AK16" ca="1" si="12">MATCH(J16,INDIRECT(J14&amp;"_L"),0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AE16" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -8934,10 +9051,10 @@
         <v>89</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="F17" s="66" t="s">
+      <c r="F17" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="66"/>
+      <c r="G17" s="69"/>
       <c r="H17" s="6"/>
       <c r="I17" s="31" t="s">
         <v>15</v>
@@ -8967,7 +9084,7 @@
         <v>63</v>
       </c>
       <c r="R17" s="8"/>
-      <c r="T17" s="67" t="s">
+      <c r="T17" s="60" t="s">
         <v>109</v>
       </c>
       <c r="U17" s="51">
@@ -8993,7 +9110,7 @@
         <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="AB17" s="73"/>
+      <c r="AB17" s="62"/>
       <c r="AC17" s="54">
         <v>10</v>
       </c>
@@ -9074,7 +9191,7 @@
         <v>0.95</v>
       </c>
       <c r="R18" s="8"/>
-      <c r="T18" s="67"/>
+      <c r="T18" s="60"/>
       <c r="U18" s="51">
         <v>21</v>
       </c>
@@ -9098,7 +9215,7 @@
         <f t="shared" ca="1" si="8"/>
         <v>106</v>
       </c>
-      <c r="AB18" s="73"/>
+      <c r="AB18" s="62"/>
       <c r="AC18" s="54">
         <v>12</v>
       </c>
@@ -9179,7 +9296,7 @@
         <v>2.23</v>
       </c>
       <c r="R19" s="8"/>
-      <c r="T19" s="67"/>
+      <c r="T19" s="60"/>
       <c r="U19" s="51">
         <v>22</v>
       </c>
@@ -9203,7 +9320,7 @@
         <f t="shared" ca="1" si="8"/>
         <v>236</v>
       </c>
-      <c r="AB19" s="73"/>
+      <c r="AB19" s="62"/>
       <c r="AC19" s="54">
         <v>16</v>
       </c>
@@ -9284,7 +9401,7 @@
         <v>70</v>
       </c>
       <c r="R20" s="8"/>
-      <c r="T20" s="67"/>
+      <c r="T20" s="60"/>
       <c r="U20" s="51">
         <v>23</v>
       </c>
@@ -9308,7 +9425,7 @@
         <f t="shared" ca="1" si="8"/>
         <v>143</v>
       </c>
-      <c r="AB20" s="74" t="s">
+      <c r="AB20" s="63" t="s">
         <v>105</v>
       </c>
       <c r="AC20" s="2">
@@ -9391,7 +9508,7 @@
         <v>1.75</v>
       </c>
       <c r="R21" s="8"/>
-      <c r="T21" s="67" t="s">
+      <c r="T21" s="60" t="s">
         <v>110</v>
       </c>
       <c r="U21" s="51">
@@ -9417,7 +9534,7 @@
         <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="AB21" s="74"/>
+      <c r="AB21" s="63"/>
       <c r="AC21" s="2">
         <v>3</v>
       </c>
@@ -9492,7 +9609,7 @@
         <v>74</v>
       </c>
       <c r="R22" s="8"/>
-      <c r="T22" s="67"/>
+      <c r="T22" s="60"/>
       <c r="U22" s="51">
         <v>25</v>
       </c>
@@ -9516,7 +9633,7 @@
         <f t="shared" ca="1" si="8"/>
         <v>146</v>
       </c>
-      <c r="AB22" s="74"/>
+      <c r="AB22" s="63"/>
       <c r="AC22" s="2">
         <v>7</v>
       </c>
@@ -9588,7 +9705,7 @@
         <v>2.17</v>
       </c>
       <c r="R23" s="8"/>
-      <c r="T23" s="67"/>
+      <c r="T23" s="60"/>
       <c r="U23" s="51">
         <v>26</v>
       </c>
@@ -9612,7 +9729,7 @@
         <f t="shared" ca="1" si="8"/>
         <v>28</v>
       </c>
-      <c r="AB23" s="74"/>
+      <c r="AB23" s="63"/>
       <c r="AC23" s="2">
         <v>10</v>
       </c>
@@ -9653,7 +9770,7 @@
       <c r="E24" s="13"/>
       <c r="F24" s="10"/>
       <c r="G24" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="31" t="s">
@@ -9684,7 +9801,7 @@
         <v>10000</v>
       </c>
       <c r="R24" s="8"/>
-      <c r="T24" s="67"/>
+      <c r="T24" s="60"/>
       <c r="U24" s="51">
         <v>27</v>
       </c>
@@ -9708,7 +9825,7 @@
         <f t="shared" ca="1" si="8"/>
         <v>131</v>
       </c>
-      <c r="AB24" s="75" t="s">
+      <c r="AB24" s="64" t="s">
         <v>106</v>
       </c>
       <c r="AC24" s="2">
@@ -9780,7 +9897,7 @@
         <v>0</v>
       </c>
       <c r="R25" s="8"/>
-      <c r="T25" s="67" t="s">
+      <c r="T25" s="60" t="s">
         <v>111</v>
       </c>
       <c r="U25" s="51">
@@ -9806,7 +9923,7 @@
         <f t="shared" si="8"/>
         <v>11</v>
       </c>
-      <c r="AB25" s="75"/>
+      <c r="AB25" s="64"/>
       <c r="AC25" s="2">
         <v>8</v>
       </c>
@@ -9858,7 +9975,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="8"/>
-      <c r="T26" s="67"/>
+      <c r="T26" s="60"/>
       <c r="U26" s="51">
         <v>29</v>
       </c>
@@ -9898,7 +10015,7 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="8"/>
-      <c r="T27" s="67"/>
+      <c r="T27" s="60"/>
       <c r="U27" s="51">
         <v>30</v>
       </c>
@@ -9922,10 +10039,10 @@
         <f t="shared" ca="1" si="8"/>
         <v>163</v>
       </c>
-      <c r="AB27" s="67" t="s">
+      <c r="AB27" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="AC27" s="67"/>
+      <c r="AC27" s="60"/>
       <c r="AD27" s="2">
         <f t="shared" ref="AD27:AK27" si="22">AD8*2^$AC8+AD9*2^$AC9+AD10*2^$AC10+AD11*2^$AC11+AD12*2^$AC12+AD13*2^$AC13</f>
         <v>531499</v>
@@ -9974,7 +10091,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="8"/>
-      <c r="T28" s="67"/>
+      <c r="T28" s="60"/>
       <c r="U28" s="51">
         <v>31</v>
       </c>
@@ -9998,13 +10115,13 @@
         <f t="shared" ca="1" si="8"/>
         <v>128</v>
       </c>
-      <c r="AB28" s="67" t="s">
+      <c r="AB28" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="AC28" s="67"/>
+      <c r="AC28" s="60"/>
       <c r="AD28" s="2">
         <f t="shared" ref="AD28:AK28" ca="1" si="23">AD14*2^$AC14+AD15*2^$AC15+AD16*2^$AC16+AD17*2^$AC17+AD18*2^$AC18+AD19*2^$AC19</f>
-        <v>14666</v>
+        <v>14537</v>
       </c>
       <c r="AE28" s="2">
         <f t="shared" ca="1" si="23"/>
@@ -10050,7 +10167,7 @@
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
       <c r="R29" s="9"/>
-      <c r="T29" s="67" t="s">
+      <c r="T29" s="60" t="s">
         <v>112</v>
       </c>
       <c r="U29" s="51">
@@ -10076,10 +10193,10 @@
         <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="AB29" s="67" t="s">
+      <c r="AB29" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="AC29" s="67"/>
+      <c r="AC29" s="60"/>
       <c r="AD29" s="2">
         <f t="shared" ref="AD29:AK29" ca="1" si="24">AD20*2^$AC20+AD21*2^$AC21+AD22*2^$AC22+AD23*2^$AC23</f>
         <v>2329</v>
@@ -10114,8 +10231,8 @@
       </c>
     </row>
     <row r="30" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="E30" s="70"/>
-      <c r="F30" s="71"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="68"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
       <c r="I30" s="17"/>
@@ -10128,7 +10245,7 @@
       <c r="P30" s="18"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="19"/>
-      <c r="T30" s="67"/>
+      <c r="T30" s="60"/>
       <c r="U30" s="51">
         <v>33</v>
       </c>
@@ -10152,10 +10269,10 @@
         <f t="shared" ca="1" si="8"/>
         <v>115</v>
       </c>
-      <c r="AB30" s="67" t="s">
+      <c r="AB30" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="AC30" s="67"/>
+      <c r="AC30" s="60"/>
       <c r="AD30" s="2">
         <f t="shared" ref="AD30:AK30" si="25">AD24*2^$AC24+AD25*2^$AC25</f>
         <v>1</v>
@@ -10204,7 +10321,7 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="8"/>
-      <c r="T31" s="67"/>
+      <c r="T31" s="60"/>
       <c r="U31" s="51">
         <v>34</v>
       </c>
@@ -10244,7 +10361,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="8"/>
-      <c r="T32" s="67"/>
+      <c r="T32" s="60"/>
       <c r="U32" s="51">
         <v>35</v>
       </c>
@@ -10288,7 +10405,7 @@
         <v>40</v>
       </c>
       <c r="R33" s="8"/>
-      <c r="T33" s="67" t="s">
+      <c r="T33" s="60" t="s">
         <v>113</v>
       </c>
       <c r="U33" s="51">
@@ -10330,7 +10447,7 @@
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
       <c r="R34" s="9"/>
-      <c r="T34" s="67"/>
+      <c r="T34" s="60"/>
       <c r="U34" s="51">
         <v>37</v>
       </c>
@@ -10356,11 +10473,11 @@
       </c>
     </row>
     <row r="35" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="E35" s="70" t="s">
+      <c r="E35" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
       <c r="H35" s="18"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
@@ -10372,7 +10489,7 @@
       <c r="P35" s="18"/>
       <c r="Q35" s="18"/>
       <c r="R35" s="19"/>
-      <c r="T35" s="67"/>
+      <c r="T35" s="60"/>
       <c r="U35" s="51">
         <v>38</v>
       </c>
@@ -10412,7 +10529,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="8"/>
-      <c r="T36" s="67"/>
+      <c r="T36" s="60"/>
       <c r="U36" s="51">
         <v>39</v>
       </c>
@@ -10432,7 +10549,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z36" s="51">
+      <c r="Z36" s="83">
         <f ca="1">_xlfn.BITXOR(Y35,Y36)</f>
         <v>133</v>
       </c>
@@ -10526,14 +10643,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AB28:AC28"/>
-    <mergeCell ref="AB29:AC29"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="AB8:AB13"/>
-    <mergeCell ref="AB14:AB19"/>
-    <mergeCell ref="AB20:AB23"/>
-    <mergeCell ref="AB24:AB25"/>
-    <mergeCell ref="AB27:AC27"/>
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="I6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="T25:T28"/>
+    <mergeCell ref="T29:T32"/>
     <mergeCell ref="T33:T36"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C16:D16"/>
@@ -10545,13 +10659,16 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="E4:R4"/>
-    <mergeCell ref="I6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="T25:T28"/>
-    <mergeCell ref="T29:T32"/>
+    <mergeCell ref="AB28:AC28"/>
+    <mergeCell ref="AB29:AC29"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AB8:AB13"/>
+    <mergeCell ref="AB14:AB19"/>
+    <mergeCell ref="AB20:AB23"/>
+    <mergeCell ref="AB24:AB25"/>
+    <mergeCell ref="AB27:AC27"/>
   </mergeCells>
-  <dataValidations count="19">
+  <dataValidations disablePrompts="1" count="19">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:Q8" xr:uid="{58ED200F-81A6-414B-9D6E-12786A48A800}">
       <formula1>RFISRC</formula1>
     </dataValidation>
@@ -10617,11 +10734,41 @@
     <ignoredError sqref="AD22:AF22" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2054" r:id="rId3" name="Button 6">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!SendCfgMsg">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>25</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>1219200</xdr:colOff>
+                    <xdr:row>28</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20645C8-7140-4786-8E03-7C126FE8C07F}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="E2:R33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -10641,22 +10788,22 @@
   <sheetData>
     <row r="2" spans="5:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="5:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="62"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="72"/>
     </row>
     <row r="4" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E4" s="13"/>
@@ -10679,17 +10826,17 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="63" t="s">
+      <c r="I5" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="65"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="75"/>
       <c r="R5" s="33"/>
     </row>
     <row r="6" spans="5:18" x14ac:dyDescent="0.25">

</xml_diff>